<commit_message>
Decreased Test Task initial OSTIMEDLYHMSM delay time
	Fixed RGB_LED Task stack size too small bug.
</commit_message>
<xml_diff>
--- a/Middlewares/FONTS/CHN.xlsx
+++ b/Middlewares/FONTS/CHN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="383">
   <si>
     <t xml:space="preserve">  ________,________,________,________,</t>
   </si>
@@ -864,6 +864,309 @@
   </si>
   <si>
     <t xml:space="preserve">  ________,________,________,_X______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____X___,________,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,_____X__,________,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,_____XXX,XXXXXXXX,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,________,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_____XX_,________,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_____XXX,XXXXXXXX,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,_____XX_,________,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XXXXXX,X____XX_,________,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XXX,XXXXXXXX,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,________,X_X_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,________,__XX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,_X______,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,__XX___X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,____XXX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,_____XXX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,____X__X,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,_XXX____,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XXX,XX______,_XXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,X____XXX,________,__XX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XXX__,_X____X_,________,___X____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XXX___,__XX_X__,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XX____,___XXXX_,________,____XXX_,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____XXXX,XXXXXXXX,XXXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,________,_XXXXXXX,XXXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_X______,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XXX_____,________,_XXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XX_____X,__X___XX,XXXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,X_____XX,X_XXXX__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XXXXX,XXXXXXXX,XXXX____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,__X_____,__XX____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,__XXX___,__XX____,____X___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______X_,__XX___X,__XXXXXX,XXXXXX__,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,__XX__XX,X_XX____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,XXXXXXXX,XXXX____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__XX____,__XX____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__XX__XX,X_XX____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,XXXXXX__,__X_____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XXXXX,X_XX____,_XX_____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XX___,__XX____,XX______,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__XX___X,X_______,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__X___X_,________,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,X_______,_______X,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XXXXXXXX,XXXXXXXX,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XX______,_______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,X_______,_______X,________,</t>
+  </si>
+  <si>
+    <t>________,________,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______X_,________,_X______,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,_XX_____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,XX______,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,XX______,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,__XXXXXX,XXXXXXXX,XXXXXX__,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,X_______,XX______,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,XX______,X___X___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___X__XX,_XX____X,X___XXX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___X__XX,__XX___X,X___XX__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___X__XX,__X____X,X___XX__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XX__XX,______XX,____XX__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XX__XX,______XX,____XX__,___X____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __X___XX,______X_,_X__XX__,__XXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,_X__XX__,_XXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,XX__XXX_,_X______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____X__,XX__XXX_,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,____XX_X,X__XX_XX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,____X___,___XX__X,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,___X____,___XX__X,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,___X____,__XX___X,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,__X_____,__XX____,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_X______,_XX_____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,X_______,_X______,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,X_______,_XXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_______X,________,__XXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,________,__XXXXX_,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,____X___,________,___X____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______X_,__XX____,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__X_____,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_XXXX___,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_XX_____,________,__XX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XXXXXXXX,XXXXXXXX,XXXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XX______,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,X_______,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_X______,_______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,_XXXXXXX,XXXXXXXX,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____XX__,_XX_____,_______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___X____,_XX_____,_______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __X_____,_XX_____,_______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_XXXXXXX,XXXXXXXX,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_XX_____,_______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_XXX____,_______X,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,___XXX__,______X_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__XX____,______XX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__XXXXXX,XXXXXXXX,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_XX_X___,_____XX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XX___X__,____XX__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,X_____X_,___XX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,______XX,_XXX____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,_______X,XXX_____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____X___,______XX,XXX_____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____XXXX,__XXXX__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__XXX___,____XXXX,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,XXX_____,______XX,XXXXXX__,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XXXX_,________,________,__XX____,</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E210"/>
+  <dimension ref="A1:E279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="C209" sqref="C208:C209"/>
+    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
+      <selection activeCell="B279" sqref="A247:B279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3035,169 +3338,796 @@
         <v>240</v>
       </c>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>0</v>
+      </c>
       <c r="B178" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="2:2">
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>0</v>
+      </c>
       <c r="B179" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="2:2">
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>0</v>
+      </c>
       <c r="B180" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="2:2">
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>282</v>
+      </c>
       <c r="B181" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="2:2">
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>283</v>
+      </c>
       <c r="B182" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="2:2">
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>284</v>
+      </c>
       <c r="B183" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="2:2">
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>285</v>
+      </c>
       <c r="B184" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="185" spans="2:2">
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>285</v>
+      </c>
       <c r="B185" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="186" spans="2:2">
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>286</v>
+      </c>
       <c r="B186" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="187" spans="2:2">
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>287</v>
+      </c>
       <c r="B187" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="188" spans="2:2">
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>286</v>
+      </c>
       <c r="B188" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="189" spans="2:2">
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>286</v>
+      </c>
       <c r="B189" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="190" spans="2:2">
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>288</v>
+      </c>
       <c r="B190" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="191" spans="2:2">
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>289</v>
+      </c>
       <c r="B191" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="192" spans="2:2">
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>290</v>
+      </c>
       <c r="B192" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="193" spans="2:2">
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>291</v>
+      </c>
       <c r="B193" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="194" spans="2:2">
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>292</v>
+      </c>
       <c r="B194" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="195" spans="2:2">
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>293</v>
+      </c>
       <c r="B195" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="2:2">
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>294</v>
+      </c>
       <c r="B196" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="2:2">
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>295</v>
+      </c>
       <c r="B197" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="198" spans="2:2">
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>296</v>
+      </c>
       <c r="B198" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="199" spans="2:2">
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>297</v>
+      </c>
       <c r="B199" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="200" spans="2:2">
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>298</v>
+      </c>
       <c r="B200" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="201" spans="2:2">
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>299</v>
+      </c>
       <c r="B201" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="202" spans="2:2">
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>300</v>
+      </c>
       <c r="B202" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="203" spans="2:2">
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>301</v>
+      </c>
       <c r="B203" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="204" spans="2:2">
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>302</v>
+      </c>
       <c r="B204" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="205" spans="2:2">
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>303</v>
+      </c>
       <c r="B205" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="206" spans="2:2">
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>304</v>
+      </c>
       <c r="B206" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="207" spans="2:2">
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>305</v>
+      </c>
       <c r="B207" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="208" spans="2:2">
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>0</v>
+      </c>
       <c r="B208" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="209" spans="2:2">
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>0</v>
+      </c>
       <c r="B209" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="2:2">
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>69</v>
+      </c>
       <c r="B210" t="s">
         <v>240</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>0</v>
+      </c>
+      <c r="B213" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>0</v>
+      </c>
+      <c r="B214" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>306</v>
+      </c>
+      <c r="B215" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>307</v>
+      </c>
+      <c r="B216" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>308</v>
+      </c>
+      <c r="B217" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>309</v>
+      </c>
+      <c r="B218" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>310</v>
+      </c>
+      <c r="B219" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>311</v>
+      </c>
+      <c r="B220" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>312</v>
+      </c>
+      <c r="B221" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>313</v>
+      </c>
+      <c r="B222" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>314</v>
+      </c>
+      <c r="B223" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>315</v>
+      </c>
+      <c r="B224" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>316</v>
+      </c>
+      <c r="B225" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>317</v>
+      </c>
+      <c r="B226" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>318</v>
+      </c>
+      <c r="B227" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>319</v>
+      </c>
+      <c r="B228" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" t="s">
+        <v>320</v>
+      </c>
+      <c r="B229" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>321</v>
+      </c>
+      <c r="B230" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>322</v>
+      </c>
+      <c r="B231" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>323</v>
+      </c>
+      <c r="B232" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>324</v>
+      </c>
+      <c r="B233" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>325</v>
+      </c>
+      <c r="B234" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>325</v>
+      </c>
+      <c r="B235" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>325</v>
+      </c>
+      <c r="B236" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>235</v>
+      </c>
+      <c r="B237" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>325</v>
+      </c>
+      <c r="B238" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>325</v>
+      </c>
+      <c r="B239" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>325</v>
+      </c>
+      <c r="B240" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>235</v>
+      </c>
+      <c r="B241" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>325</v>
+      </c>
+      <c r="B242" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>326</v>
+      </c>
+      <c r="B243" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>0</v>
+      </c>
+      <c r="B244" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>69</v>
+      </c>
+      <c r="B245" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>327</v>
+      </c>
+      <c r="B247" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>0</v>
+      </c>
+      <c r="B248" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>328</v>
+      </c>
+      <c r="B249" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>329</v>
+      </c>
+      <c r="B250" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>330</v>
+      </c>
+      <c r="B251" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" t="s">
+        <v>330</v>
+      </c>
+      <c r="B252" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" t="s">
+        <v>331</v>
+      </c>
+      <c r="B253" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" t="s">
+        <v>332</v>
+      </c>
+      <c r="B254" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" t="s">
+        <v>333</v>
+      </c>
+      <c r="B255" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>334</v>
+      </c>
+      <c r="B256" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>335</v>
+      </c>
+      <c r="B257" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>336</v>
+      </c>
+      <c r="B258" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>337</v>
+      </c>
+      <c r="B259" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>338</v>
+      </c>
+      <c r="B260" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>339</v>
+      </c>
+      <c r="B261" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>340</v>
+      </c>
+      <c r="B262" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>341</v>
+      </c>
+      <c r="B263" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>342</v>
+      </c>
+      <c r="B264" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" t="s">
+        <v>343</v>
+      </c>
+      <c r="B265" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266" t="s">
+        <v>344</v>
+      </c>
+      <c r="B266" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" t="s">
+        <v>345</v>
+      </c>
+      <c r="B267" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268" t="s">
+        <v>346</v>
+      </c>
+      <c r="B268" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269" t="s">
+        <v>347</v>
+      </c>
+      <c r="B269" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270" t="s">
+        <v>348</v>
+      </c>
+      <c r="B270" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" t="s">
+        <v>349</v>
+      </c>
+      <c r="B271" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="A272" t="s">
+        <v>350</v>
+      </c>
+      <c r="B272" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273" t="s">
+        <v>351</v>
+      </c>
+      <c r="B273" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>352</v>
+      </c>
+      <c r="B274" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
+        <v>353</v>
+      </c>
+      <c r="B275" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
+        <v>354</v>
+      </c>
+      <c r="B276" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>355</v>
+      </c>
+      <c r="B277" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>0</v>
+      </c>
+      <c r="B278" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279" t="s">
+        <v>69</v>
+      </c>
+      <c r="B279" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved Font bmp to a individual file
</commit_message>
<xml_diff>
--- a/Middlewares/FONTS/CHN.xlsx
+++ b/Middlewares/FONTS/CHN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="521">
   <si>
     <t xml:space="preserve">  ________,________,________,________,</t>
   </si>
@@ -1167,6 +1167,422 @@
   </si>
   <si>
     <t xml:space="preserve">  ___XXXX_,________,________,__XX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XXXXXX,XXXXXXXX,X_______,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,________,__X_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX_X,XXXXXXXX,XXXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,_X______,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,__X_____,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,XXXXXX__,__X_____,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,__X_____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,___X____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,___X___X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,XXXXXX__,___X___X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,___XX__X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,____X_XX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,____XXXX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____XX__,XX__XXX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,___XXXXX,_____XX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,XXX_XX__,____XXX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XXXXXX,____XX__,____XXXX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XXX___,____XX__,___XX__X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____XX__,__XX____,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____XX__,__X_____,_XXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____XX__,_X______,__XXXXX_,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____XX__,X_______,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____XX_X,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____X_X_,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,________,___XX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,________,___XXX__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______X_,_____X__,___XX___,__XX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,X____XXX,___XX___,__XX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,X_____XX,X__XX___,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,X______X,X__XX___,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,___X___X,X__XX___,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,___X____,___XX__X,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __X_____,___X_X__,___XX___,__X_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XX___,__X__XXX,XXXXXXXX,XXXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XXX__,__X__XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____XX__,__X__XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,_X___XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_X___XXX,XXXXXXXX,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XX___XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,X____XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,X____XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XXX,XXXXXXXX,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XXXXXX,_____XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,_____XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,_____XX_,_____XXX,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____XX_,________,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_____X__,________,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,________,________,________</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,________,________,________,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,________,__XX____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,________,__XXX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,________,_XX_____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,___XX___,_XX_____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XXXXXX,XXXXXX__,XXXXXXXX,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,X______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_______X,X______X,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_______X,______X_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______X_,______XX,_____X__,___X____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,_____X_X,XXXXXXXX,XXXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XX_,____X__X,X____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,__XX___X,X____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____XXXX,XXXXX__X,X____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____XX__,__XX___X,X____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____XX__,__XX___X,XXXXXXXX,XXXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___X_X__,__XX___X,X____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __X__X__,__XX___X,X____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _X___X__,__XX___X,X____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,__XX___X,XXXXXXXX,XXXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,__XX___X,_____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,XXXX__XX,_____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,__XX__XX,_____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,______X_,_____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____X__,_____XX_,_____XX_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_____X__,_____XXX,XXXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____X___,_____X__,__XX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,___X____,________,__X_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,________,___X____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,___XX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,XX______,___XX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XX______,__XXX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,X_______,__XXX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,________,__XXX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,X_______,__XXX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XXXX_X,X_______,__XXX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,________,__XX_X__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,________,__X__X__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,________,_XX__X__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,________,_XX__XX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,_____X__,_XX___X_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,____X___,XX____XX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,___X____,XX_____X,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,__X____X,X______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,_XX____X,_______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,XX____XX,________,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,X____XX_,________,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,____X___,________,_XXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__XX____,________,__XXXX__,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_XX_____,________,___X____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,X_______,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,__XXX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,_XX_X___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,_XX__X__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,_X___XX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,___X____,XX____XX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _XXXXXXX,XXXXX__X,X______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_______X,________,XXX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,______X_,________,_XXXX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_____X__,________,__XXXX__,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,X___X___,_______X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,_XXX__XX,XXXXXXXX,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,__XX____,________,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _____XXX,__XX____,________,_X______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____XXXX,___X____,__X_____,_XX_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____X_XX,_____X__,__XX____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XX_XX,_____X__,___X____,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___X__XX,______X_,___XX___,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __X___XX,______XX,___XX___,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _X____XX,_______X,___XX__X,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_______X,X___X__X,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,_______X,______XX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,______X_,___XX___,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,________,______X_,__XXXX__,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,___XXXXX,XXXXXX_X,XX______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XXXXX,XXXXXXXX,XXXXXXXX,XXXXXX__,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_____XXX,X_X_____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,_____XXX,X__X____,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,____XX_X,X__XX___,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,___XX__X,X___XX__,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,__XX___X,X____XX_,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,XXX____X,X_____XX,X_______,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  _______X,X______X,X______X,XXXX____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ______XX,X_____X_,_______X,_XXXXX__,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ____XX__,XXXXXXXX,XXXXXXXX,X__X____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  __XX____,XX______,______XX,________,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ________,X_______,________,__X_____,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ___XXXXX,XXXXXXXX,XXXXXXXX,XXXXX___,</t>
   </si>
 </sst>
 </file>
@@ -1510,15 +1926,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E279"/>
+  <dimension ref="A1:E384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="B279" sqref="A247:B279"/>
+    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="B352" sqref="B352:B384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="42.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.75" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="43.875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="42.75" bestFit="1" customWidth="1"/>
   </cols>
@@ -4127,6 +4543,798 @@
         <v>69</v>
       </c>
       <c r="B279" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282" t="s">
+        <v>0</v>
+      </c>
+      <c r="B282" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283" t="s">
+        <v>0</v>
+      </c>
+      <c r="B283" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="A284" t="s">
+        <v>0</v>
+      </c>
+      <c r="B284" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285" t="s">
+        <v>97</v>
+      </c>
+      <c r="B285" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" t="s">
+        <v>383</v>
+      </c>
+      <c r="B286" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="A287" t="s">
+        <v>384</v>
+      </c>
+      <c r="B287" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288" t="s">
+        <v>385</v>
+      </c>
+      <c r="B288" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="A289" t="s">
+        <v>386</v>
+      </c>
+      <c r="B289" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290" t="s">
+        <v>387</v>
+      </c>
+      <c r="B290" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="A291" t="s">
+        <v>388</v>
+      </c>
+      <c r="B291" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
+      <c r="A292" t="s">
+        <v>389</v>
+      </c>
+      <c r="B292" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2">
+      <c r="A293" t="s">
+        <v>388</v>
+      </c>
+      <c r="B293" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
+      <c r="A294" t="s">
+        <v>390</v>
+      </c>
+      <c r="B294" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
+      <c r="A295" t="s">
+        <v>390</v>
+      </c>
+      <c r="B295" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
+      <c r="A296" t="s">
+        <v>391</v>
+      </c>
+      <c r="B296" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297" t="s">
+        <v>392</v>
+      </c>
+      <c r="B297" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
+      <c r="A298" t="s">
+        <v>393</v>
+      </c>
+      <c r="B298" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
+      <c r="A299" t="s">
+        <v>394</v>
+      </c>
+      <c r="B299" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300" t="s">
+        <v>395</v>
+      </c>
+      <c r="B300" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
+      <c r="A301" t="s">
+        <v>396</v>
+      </c>
+      <c r="B301" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
+      <c r="A302" t="s">
+        <v>397</v>
+      </c>
+      <c r="B302" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2">
+      <c r="A303" t="s">
+        <v>398</v>
+      </c>
+      <c r="B303" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="A304" t="s">
+        <v>399</v>
+      </c>
+      <c r="B304" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
+      <c r="A305" t="s">
+        <v>400</v>
+      </c>
+      <c r="B305" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2">
+      <c r="A306" t="s">
+        <v>401</v>
+      </c>
+      <c r="B306" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2">
+      <c r="A307" t="s">
+        <v>402</v>
+      </c>
+      <c r="B307" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2">
+      <c r="A308" t="s">
+        <v>403</v>
+      </c>
+      <c r="B308" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2">
+      <c r="A309" t="s">
+        <v>404</v>
+      </c>
+      <c r="B309" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2">
+      <c r="A310" t="s">
+        <v>405</v>
+      </c>
+      <c r="B310" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2">
+      <c r="A311" t="s">
+        <v>406</v>
+      </c>
+      <c r="B311" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2">
+      <c r="A312" t="s">
+        <v>407</v>
+      </c>
+      <c r="B312" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2">
+      <c r="A313" t="s">
+        <v>0</v>
+      </c>
+      <c r="B313" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2">
+      <c r="A314" t="s">
+        <v>433</v>
+      </c>
+      <c r="B314" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2">
+      <c r="A317" t="s">
+        <v>0</v>
+      </c>
+      <c r="B317" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2">
+      <c r="A318" t="s">
+        <v>0</v>
+      </c>
+      <c r="B318" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2">
+      <c r="A319" t="s">
+        <v>434</v>
+      </c>
+      <c r="B319" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2">
+      <c r="A320" t="s">
+        <v>435</v>
+      </c>
+      <c r="B320" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" t="s">
+        <v>436</v>
+      </c>
+      <c r="B321" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="A322" t="s">
+        <v>437</v>
+      </c>
+      <c r="B322" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2">
+      <c r="A323" t="s">
+        <v>438</v>
+      </c>
+      <c r="B323" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2">
+      <c r="A324" t="s">
+        <v>439</v>
+      </c>
+      <c r="B324" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2">
+      <c r="A325" t="s">
+        <v>440</v>
+      </c>
+      <c r="B325" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="A326" t="s">
+        <v>441</v>
+      </c>
+      <c r="B326" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="A327" t="s">
+        <v>442</v>
+      </c>
+      <c r="B327" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="A328" t="s">
+        <v>443</v>
+      </c>
+      <c r="B328" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2">
+      <c r="A329" t="s">
+        <v>444</v>
+      </c>
+      <c r="B329" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="A330" t="s">
+        <v>445</v>
+      </c>
+      <c r="B330" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
+      <c r="A331" t="s">
+        <v>446</v>
+      </c>
+      <c r="B331" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
+      <c r="A332" t="s">
+        <v>447</v>
+      </c>
+      <c r="B332" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="A333" t="s">
+        <v>448</v>
+      </c>
+      <c r="B333" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" t="s">
+        <v>449</v>
+      </c>
+      <c r="B334" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="A335" t="s">
+        <v>449</v>
+      </c>
+      <c r="B335" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" t="s">
+        <v>450</v>
+      </c>
+      <c r="B336" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
+      <c r="A337" t="s">
+        <v>451</v>
+      </c>
+      <c r="B337" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
+      <c r="A338" t="s">
+        <v>452</v>
+      </c>
+      <c r="B338" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2">
+      <c r="A339" t="s">
+        <v>445</v>
+      </c>
+      <c r="B339" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
+      <c r="A340" t="s">
+        <v>453</v>
+      </c>
+      <c r="B340" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2">
+      <c r="A341" t="s">
+        <v>454</v>
+      </c>
+      <c r="B341" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2">
+      <c r="A342" t="s">
+        <v>455</v>
+      </c>
+      <c r="B342" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2">
+      <c r="A343" t="s">
+        <v>456</v>
+      </c>
+      <c r="B343" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
+      <c r="A344" t="s">
+        <v>457</v>
+      </c>
+      <c r="B344" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2">
+      <c r="A345" t="s">
+        <v>458</v>
+      </c>
+      <c r="B345" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2">
+      <c r="A346" t="s">
+        <v>459</v>
+      </c>
+      <c r="B346" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
+      <c r="A347" t="s">
+        <v>460</v>
+      </c>
+      <c r="B347" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2">
+      <c r="A348" t="s">
+        <v>0</v>
+      </c>
+      <c r="B348" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2">
+      <c r="A349" t="s">
+        <v>433</v>
+      </c>
+      <c r="B349" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
+      <c r="A352" t="s">
+        <v>0</v>
+      </c>
+      <c r="B352" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="A353" t="s">
+        <v>0</v>
+      </c>
+      <c r="B353" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2">
+      <c r="A354" t="s">
+        <v>177</v>
+      </c>
+      <c r="B354" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2">
+      <c r="A355" t="s">
+        <v>467</v>
+      </c>
+      <c r="B355" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
+      <c r="A356" t="s">
+        <v>484</v>
+      </c>
+      <c r="B356" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
+      <c r="A357" t="s">
+        <v>485</v>
+      </c>
+      <c r="B357" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2">
+      <c r="A358" t="s">
+        <v>486</v>
+      </c>
+      <c r="B358" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2">
+      <c r="A359" t="s">
+        <v>487</v>
+      </c>
+      <c r="B359" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2">
+      <c r="A360" t="s">
+        <v>488</v>
+      </c>
+      <c r="B360" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
+      <c r="A361" t="s">
+        <v>489</v>
+      </c>
+      <c r="B361" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2">
+      <c r="A362" t="s">
+        <v>490</v>
+      </c>
+      <c r="B362" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
+      <c r="A363" t="s">
+        <v>491</v>
+      </c>
+      <c r="B363" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="A364" t="s">
+        <v>492</v>
+      </c>
+      <c r="B364" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
+      <c r="A365" t="s">
+        <v>493</v>
+      </c>
+      <c r="B365" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
+      <c r="A366" t="s">
+        <v>494</v>
+      </c>
+      <c r="B366" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
+      <c r="A367" t="s">
+        <v>495</v>
+      </c>
+      <c r="B367" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
+      <c r="A368" t="s">
+        <v>496</v>
+      </c>
+      <c r="B368" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2">
+      <c r="A369" t="s">
+        <v>497</v>
+      </c>
+      <c r="B369" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" t="s">
+        <v>498</v>
+      </c>
+      <c r="B370" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2">
+      <c r="A371" t="s">
+        <v>499</v>
+      </c>
+      <c r="B371" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" t="s">
+        <v>500</v>
+      </c>
+      <c r="B372" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
+      <c r="A373" t="s">
+        <v>501</v>
+      </c>
+      <c r="B373" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2">
+      <c r="A374" t="s">
+        <v>501</v>
+      </c>
+      <c r="B374" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2">
+      <c r="A375" t="s">
+        <v>502</v>
+      </c>
+      <c r="B375" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" t="s">
+        <v>503</v>
+      </c>
+      <c r="B376" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2">
+      <c r="A377" t="s">
+        <v>440</v>
+      </c>
+      <c r="B377" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" t="s">
+        <v>504</v>
+      </c>
+      <c r="B378" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" t="s">
+        <v>505</v>
+      </c>
+      <c r="B379" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" t="s">
+        <v>506</v>
+      </c>
+      <c r="B380" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" t="s">
+        <v>507</v>
+      </c>
+      <c r="B381" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" t="s">
+        <v>246</v>
+      </c>
+      <c r="B382" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2">
+      <c r="A383" t="s">
+        <v>0</v>
+      </c>
+      <c r="B383" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" t="s">
+        <v>433</v>
+      </c>
+      <c r="B384" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>